<commit_message>
Remove <br> from metadata
</commit_message>
<xml_diff>
--- a/automation/schulferien/metadata_ferientermine_volksschule.xlsx
+++ b/automation/schulferien/metadata_ferientermine_volksschule.xlsx
@@ -1019,9 +1019,9 @@
     <t>Datum der Erstellung des Kalendereintrags</t>
   </si>
   <si>
-    <t xml:space="preserve">410.1 Bildungsgesetz (BiG) §7 &lt;br&gt;
-412.100 Volksschulgesetz (VSG) § 30 &lt;br&gt;
-412.101 Volksschulverordnung (VSV) § 32 &lt;br&gt;
+    <t xml:space="preserve">410.1 Bildungsgesetz (BiG) §7 
+412.100 Volksschulgesetz (VSG) § 30 
+412.101 Volksschulverordnung (VSV) § 32 
 412.31 Lehrpersonalgesetz (LPG) § 23 Abs. 3
 </t>
   </si>
@@ -1756,7 +1756,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2961,21 +2961,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3089,17 +3074,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3113,17 +3114,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>